<commit_message>
fix 9mm damage 3
</commit_message>
<xml_diff>
--- a/changes/9mm-ammo.xlsx
+++ b/changes/9mm-ammo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1105D03-35C0-4437-B91B-81D4D58887ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F21BAB-85DC-4380-984F-80EB7C485C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1041,7 +1041,7 @@
   <dimension ref="A1:AJ16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,7 +1754,7 @@
         <v>0.05</v>
       </c>
       <c r="I12">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="J12">
         <v>-150</v>
@@ -1805,7 +1805,7 @@
         <v>0.1</v>
       </c>
       <c r="I13">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="J13">
         <v>0</v>

</xml_diff>

<commit_message>
fix makarov laser, adjust 9mm ammo
</commit_message>
<xml_diff>
--- a/changes/9mm-ammo.xlsx
+++ b/changes/9mm-ammo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F3454FA-9537-4684-AEC4-44B1D113EBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E811619B-070A-4CC6-8FCC-A70BCB2E5458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>new</t>
   </si>
@@ -720,7 +720,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1055,7 +1083,7 @@
   <dimension ref="A1:AJ23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,8 +1721,14 @@
       <c r="S10" t="s">
         <v>38</v>
       </c>
+      <c r="T10" t="s">
+        <v>33</v>
+      </c>
       <c r="U10" t="s">
         <v>31</v>
+      </c>
+      <c r="V10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1711,13 +1745,13 @@
         <v>0.02</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F11">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H11">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J11">
         <v>-100</v>
@@ -1726,8 +1760,8 @@
         <v>2000</v>
       </c>
       <c r="N11">
-        <f>C11-D11*20-E11*0.8-F11*0.6-H11*5+(U11-25)*1.5+J11/300+S11*2+R11/2</f>
-        <v>12.656666666666666</v>
+        <f t="shared" ref="N11:N16" si="3">C11-D11*20-E11*0.8-F11*0.6-H11*5+(AVERAGE(T11:V11)-25)*2+J11/300+S11*2+R11/2</f>
+        <v>16.889999999999997</v>
       </c>
       <c r="P11">
         <v>1150</v>
@@ -1741,44 +1775,53 @@
       <c r="S11">
         <v>0.02</v>
       </c>
+      <c r="T11">
+        <v>50</v>
+      </c>
       <c r="U11">
         <v>45</v>
+      </c>
+      <c r="V11">
+        <v>39</v>
+      </c>
+      <c r="W11" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>-1</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
       <c r="H12">
-        <v>0.05</v>
+        <v>-0.05</v>
       </c>
       <c r="I12">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
       <c r="J12">
         <v>-150</v>
       </c>
       <c r="M12">
-        <v>750</v>
+        <v>1500</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N16" si="3">C12-D12*20-E12*0.8-F12*0.6-H12*5+(U12-25)*1.5+J12/300+S12*2+R12/2</f>
-        <v>12.799999999999999</v>
+        <f t="shared" si="3"/>
+        <v>16.533333333333328</v>
       </c>
       <c r="P12">
         <v>1100</v>
@@ -1792,8 +1835,17 @@
       <c r="S12">
         <v>0.1</v>
       </c>
+      <c r="T12">
+        <v>41</v>
+      </c>
       <c r="U12">
         <v>34</v>
+      </c>
+      <c r="V12">
+        <v>26</v>
+      </c>
+      <c r="W12" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -1816,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0.02</v>
@@ -1829,7 +1881,7 @@
       </c>
       <c r="N13">
         <f t="shared" si="3"/>
-        <v>11.25</v>
+        <v>15.25</v>
       </c>
       <c r="P13">
         <v>1250</v>
@@ -1843,44 +1895,53 @@
       <c r="S13">
         <v>0.2</v>
       </c>
+      <c r="T13">
+        <v>39</v>
+      </c>
       <c r="U13">
         <v>32</v>
+      </c>
+      <c r="V13">
+        <v>25</v>
+      </c>
+      <c r="W13" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="E14">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="F14">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="H14">
-        <v>-0.05</v>
+        <v>0.05</v>
       </c>
       <c r="I14">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="J14">
         <v>-150</v>
       </c>
       <c r="M14">
-        <v>1500</v>
+        <v>750</v>
       </c>
       <c r="N14">
         <f t="shared" si="3"/>
-        <v>14.98</v>
+        <v>15.613333333333337</v>
       </c>
       <c r="P14">
         <v>1100</v>
@@ -1894,8 +1955,17 @@
       <c r="S14">
         <v>0.09</v>
       </c>
+      <c r="T14">
+        <v>37</v>
+      </c>
       <c r="U14">
         <v>31</v>
+      </c>
+      <c r="V14">
+        <v>24</v>
+      </c>
+      <c r="W14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
@@ -1906,13 +1976,13 @@
         <v>49</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="F15">
         <v>-3</v>
@@ -1931,7 +2001,7 @@
       </c>
       <c r="N15">
         <f t="shared" si="3"/>
-        <v>14.670000000000002</v>
+        <v>15.136666666666667</v>
       </c>
       <c r="P15">
         <v>1250</v>
@@ -1945,8 +2015,17 @@
       <c r="S15">
         <v>0.11</v>
       </c>
+      <c r="T15">
+        <v>33</v>
+      </c>
       <c r="U15">
         <v>29</v>
+      </c>
+      <c r="V15">
+        <v>23</v>
+      </c>
+      <c r="W15" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
@@ -1957,7 +2036,7 @@
         <v>51</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16">
         <v>0.06</v>
@@ -1966,7 +2045,7 @@
         <v>-8</v>
       </c>
       <c r="F16">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="H16">
         <v>0.2</v>
@@ -1982,7 +2061,7 @@
       </c>
       <c r="N16">
         <f t="shared" si="3"/>
-        <v>15.290000000000003</v>
+        <v>15.89</v>
       </c>
       <c r="P16">
         <v>950</v>
@@ -1996,14 +2075,20 @@
       <c r="S16">
         <v>0.02</v>
       </c>
+      <c r="T16">
+        <v>33</v>
+      </c>
       <c r="U16">
         <v>27</v>
       </c>
+      <c r="V16">
+        <v>21</v>
+      </c>
+      <c r="W16" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="18" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P18">
-        <v>1150</v>
-      </c>
+    <row r="18" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q18">
         <v>60</v>
       </c>
@@ -2014,10 +2099,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P19">
-        <v>1100</v>
-      </c>
+    <row r="19" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q19">
         <v>50</v>
       </c>
@@ -2028,10 +2110,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P20">
-        <v>1250</v>
-      </c>
+    <row r="20" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q20">
         <v>70</v>
       </c>
@@ -2042,10 +2121,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P21">
-        <v>1100</v>
-      </c>
+    <row r="21" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q21">
         <v>50</v>
       </c>
@@ -2056,10 +2132,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="22" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P22">
-        <v>1250</v>
-      </c>
+    <row r="22" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q22">
         <v>70</v>
       </c>
@@ -2070,10 +2143,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="16:19" x14ac:dyDescent="0.25">
-      <c r="P23">
-        <v>950</v>
-      </c>
+    <row r="23" spans="17:19" x14ac:dyDescent="0.25">
       <c r="Q23">
         <v>80</v>
       </c>
@@ -2085,9 +2155,34 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C11:D16 G11:O16 Q11:U16">
+  <conditionalFormatting sqref="C11:D11 C13:D13 G11:O11 G13:M13 T11:V12 T15:V16 G15:M16 O15:O16 O13 N11:N16">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C11&lt;&gt;C3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T14:V14">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>T14&lt;&gt;T5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15:D16">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>C15&lt;&gt;C7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T14:V14 C14:D14 G14:M14 O14">
+    <cfRule type="expression" dxfId="4" priority="7">
+      <formula>C14&lt;&gt;C4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T13:V13">
+    <cfRule type="expression" dxfId="3" priority="8">
+      <formula>T13&lt;&gt;T5</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:D12 G12:M12 O12">
+    <cfRule type="expression" dxfId="2" priority="10">
+      <formula>C12&lt;&gt;C6</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>